<commit_message>
Documentacion: aplicadas sugerencias Paco
</commit_message>
<xml_diff>
--- a/doc/imagenes/facerecognition-results-num-nodes.xlsx
+++ b/doc/imagenes/facerecognition-results-num-nodes.xlsx
@@ -177,17 +177,20 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$D$10:$F$10</c:f>
+              <c:f>Hoja1!$D$10:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -195,10 +198,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$11:$F$11</c:f>
+              <c:f>Hoja1!$D$11:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>44.5</c:v>
                 </c:pt>
@@ -206,6 +209,9 @@
                   <c:v>44.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>44.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>44.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -232,17 +238,20 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$D$10:$F$10</c:f>
+              <c:f>Hoja1!$D$10:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -250,18 +259,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$12:$F$12</c:f>
+              <c:f>Hoja1!$D$12:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>25.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.5</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.333333333333333</c:v>
+                  <c:v>13.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.833333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -287,17 +299,20 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$D$10:$F$10</c:f>
+              <c:f>Hoja1!$D$10:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -305,17 +320,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$13:$F$13</c:f>
+              <c:f>Hoja1!$D$13:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>25.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>11.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6.4</c:v>
                 </c:pt>
               </c:numCache>
@@ -332,11 +350,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2099379376"/>
-        <c:axId val="2099346880"/>
+        <c:axId val="2119671248"/>
+        <c:axId val="2119680800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099379376"/>
+        <c:axId val="2119671248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,7 +390,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099346880"/>
+        <c:crossAx val="2119680800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -380,7 +398,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099346880"/>
+        <c:axId val="2119680800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,7 +436,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099379376"/>
+        <c:crossAx val="2119671248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -489,7 +507,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$D$10:$F$10</c:f>
+              <c:f>Hoja1!$E$10:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -507,7 +525,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$11:$F$11</c:f>
+              <c:f>Hoja1!$E$11:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -544,7 +562,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$D$10:$F$10</c:f>
+              <c:f>Hoja1!$E$10:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -562,7 +580,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$13:$F$13</c:f>
+              <c:f>Hoja1!$E$13:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -589,11 +607,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2099326544"/>
-        <c:axId val="2099401776"/>
+        <c:axId val="2119583328"/>
+        <c:axId val="2101652896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099326544"/>
+        <c:axId val="2119583328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099401776"/>
+        <c:crossAx val="2101652896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -637,7 +655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099401776"/>
+        <c:axId val="2101652896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -675,7 +693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099326544"/>
+        <c:crossAx val="2119583328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -707,7 +725,7 @@
       <xdr:rowOff>27940</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>314960</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>27940</xdr:rowOff>
@@ -731,7 +749,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>20320</xdr:rowOff>
@@ -784,7 +802,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>294640</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>193040</xdr:rowOff>
@@ -837,7 +855,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>162560</xdr:rowOff>
@@ -890,13 +908,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>772160</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -922,7 +940,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>314960</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
@@ -975,7 +993,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>345440</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
@@ -1351,37 +1369,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:H19"/>
+  <dimension ref="C6:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="3" max="4" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>2</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>4</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>3</v>
       </c>
@@ -1394,39 +1415,49 @@
       <c r="F11">
         <v>44.5</v>
       </c>
+      <c r="G11">
+        <v>44.5</v>
+      </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E12">
         <f>D12/2</f>
-        <v>12.5</v>
+        <v>26.5</v>
       </c>
       <c r="F12">
-        <f>D12/3</f>
-        <v>8.3333333333333339</v>
+        <f>D12/4</f>
+        <v>13.25</v>
+      </c>
+      <c r="G12">
+        <f>D12/6</f>
+        <v>8.8333333333333339</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="D13">
+        <v>53</v>
+      </c>
+      <c r="E13">
         <v>25</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>11.5</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>6.4</v>
       </c>
     </row>
-    <row r="19" spans="8:8" ht="28" x14ac:dyDescent="0.3">
-      <c r="H19" s="1"/>
+    <row r="19" spans="9:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="I19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>